<commit_message>
Update BAU production/imports/exports to set lignite and natural gas exports to 0 and to customize balancing priorities
</commit_message>
<xml_diff>
--- a/InputData/fuels/FPIEBP/Fuel Prod Imp Exp Balancing Priorities.xlsx
+++ b/InputData/fuels/FPIEBP/Fuel Prod Imp Exp Balancing Priorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\fuels\FPIEBP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\fuels\FPIEBP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4E0A33-3857-4E42-99DE-F3DBB58130FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F37C51-9B5F-4506-AB54-A0BA8DECD4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18705" yWindow="1695" windowWidth="19470" windowHeight="20340" xr2:uid="{B505BEC9-7B7D-48ED-A025-9B3B4252ED08}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B505BEC9-7B7D-48ED-A025-9B3B4252ED08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -616,16 +616,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290315BF-FDD8-4070-97AB-AF459B926789}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,90 +635,90 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -724,97 +726,97 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -832,15 +834,18 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="4" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="4" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
@@ -854,7 +859,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -868,35 +873,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -910,7 +915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
@@ -924,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
@@ -938,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -952,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -967,77 +972,77 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="C10" s="9">
-        <v>3</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>3</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9">
-        <v>3</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="9">
-        <v>1</v>
-      </c>
-      <c r="C14" s="9">
-        <v>3</v>
-      </c>
-      <c r="D14" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>51</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>52</v>
       </c>
@@ -1065,21 +1070,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="9">
-        <v>1</v>
-      </c>
-      <c r="C17" s="9">
-        <v>3</v>
-      </c>
-      <c r="D17" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -1093,60 +1098,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="9">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9">
-        <v>3</v>
-      </c>
-      <c r="D19" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="9">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9">
-        <v>3</v>
-      </c>
-      <c r="D20" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9">
-        <v>3</v>
-      </c>
-      <c r="D21" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="9">
-        <v>1</v>
+      <c r="B22">
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>